<commit_message>
Correction s_vs_i valeur temporelle de s+ et s-
</commit_message>
<xml_diff>
--- a/Distribution spatiale de l'intensité du jet atomique non-défléchi.xlsx
+++ b/Distribution spatiale de l'intensité du jet atomique non-défléchi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NYCbo\PycharmProjects\S&amp;G\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NYCbo\OneDrive\Documents\GitHub\S-G\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E32DF4-AEF9-49E4-B8E1-CD930C178E4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C118CD-0FF6-4DBF-9CF5-69A65BE47717}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8A1DECB7-6969-4ABC-82D1-218CE757C469}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Figure</t>
   </si>
@@ -80,18 +80,12 @@
     <t>s- [s]</t>
   </si>
   <si>
-    <t>s [m]</t>
-  </si>
-  <si>
     <t>t0 [s]</t>
   </si>
   <si>
     <t>t0'[s]</t>
   </si>
   <si>
-    <t>Incertitude s [m]</t>
-  </si>
-  <si>
     <t>Incertitude B moyen</t>
   </si>
   <si>
@@ -99,6 +93,24 @@
   </si>
   <si>
     <t>|s-| [s]</t>
+  </si>
+  <si>
+    <t>s+ [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>distance parcourue par le moteur :</t>
+  </si>
+  <si>
+    <t>s [mm]</t>
+  </si>
+  <si>
+    <t>s-[mm]</t>
+  </si>
+  <si>
+    <t>Incertitude s [mm]</t>
   </si>
 </sst>
 </file>
@@ -450,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF01328-6455-46C0-A076-C89038FA0C70}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,13 +478,15 @@
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="31" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" customWidth="1"/>
     <col min="13" max="13" width="20.140625" customWidth="1"/>
     <col min="14" max="14" width="17.140625" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,8 +511,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -523,8 +543,11 @@
       <c r="H2">
         <v>4.78</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>25.552399999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -550,7 +573,7 @@
         <v>9.7899999999999991</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -576,7 +599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -602,7 +625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -628,7 +651,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -654,7 +677,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -680,7 +703,7 @@
         <v>7.81</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -697,37 +720,43 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
       </c>
       <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
         <v>8</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>10</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>12</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" t="s">
         <v>18</v>
       </c>
-      <c r="M12" t="s">
+      <c r="Q12" t="s">
         <v>19</v>
       </c>
-      <c r="N12" t="s">
-        <v>20</v>
-      </c>
-      <c r="O12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -744,43 +773,51 @@
         <v>-7.0640000000000001</v>
       </c>
       <c r="F13">
+        <f>(D13 * $K$2)/(I13-H13)</f>
+        <v>2.6524209527359259</v>
+      </c>
+      <c r="G13">
+        <f>(Q13 * $K$2)/(I13-H13)</f>
+        <v>2.5875848101265819</v>
+      </c>
+      <c r="H13">
         <v>25.783000000000001</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>95.54</v>
       </c>
-      <c r="H13">
-        <f xml:space="preserve"> (((D13-E13)/2)*25.5524)/(G13-F13)</f>
+      <c r="J13">
+        <f xml:space="preserve"> (((D13-E13)/2)*25.5524)/(I13-H13)</f>
         <v>2.6200028814312537</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <f xml:space="preserve"> (93.139/ 100*80.99)/85.25</f>
         <v>0.88484781348973596</v>
       </c>
-      <c r="J13">
-        <f xml:space="preserve"> 5.5 *0.1* I13</f>
+      <c r="L13">
+        <f xml:space="preserve"> 5.5 *0.1* K13</f>
         <v>0.4866662974193548</v>
       </c>
-      <c r="K13">
-        <f>(L13*I13)/H13</f>
+      <c r="M13">
+        <f>(N13*K13)/J13</f>
         <v>6.1855841558177978E-2</v>
       </c>
-      <c r="L13">
-        <f>((0.5*25.5524)/(G13-F13))</f>
+      <c r="N13">
+        <f>((0.5*25.5524)/(I13-H13))</f>
         <v>0.18315294522413519</v>
       </c>
-      <c r="M13">
-        <f>(K13*J13)/I13</f>
+      <c r="O13">
+        <f>(M13*L13)/K13</f>
         <v>3.4020712856997891E-2</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>0.5</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>7.0640000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -797,43 +834,51 @@
         <v>-6.8879999999999999</v>
       </c>
       <c r="F14">
+        <f t="shared" ref="F14:F19" si="0">(D14 * $K$2)/(I14-H14)</f>
+        <v>2.6004149849430136</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G19" si="1">(Q14 * $K$2)/(I14-H14)</f>
+        <v>2.5359844848205406</v>
+      </c>
+      <c r="H14">
         <v>10.419</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>79.822000000000003</v>
       </c>
-      <c r="H14">
-        <f xml:space="preserve"> (((D14-E14)/2)*25.5524)/(G14-F14)</f>
+      <c r="J14">
+        <f xml:space="preserve"> (((D14-E14)/2)*25.5524)/(I14-H14)</f>
         <v>2.5681997348817771</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <f xml:space="preserve"> (91.298 / 100*80.99)/85.25</f>
         <v>0.86735777360703803</v>
       </c>
-      <c r="J14">
-        <f t="shared" ref="J14:J19" si="0" xml:space="preserve"> 5.5 *0.1* I14</f>
+      <c r="L14">
+        <f t="shared" ref="L14:L19" si="2" xml:space="preserve"> 5.5 *0.1* K14</f>
         <v>0.47704677548387098</v>
       </c>
-      <c r="K14">
-        <f t="shared" ref="K14:K19" si="1">(L14*I14)/H14</f>
+      <c r="M14">
+        <f t="shared" ref="M14:M19" si="3">(N14*K14)/J14</f>
         <v>6.2171727733283499E-2</v>
       </c>
-      <c r="L14">
-        <f t="shared" ref="L14:L19" si="2">((0.5*25.5524)/(G14-F14))</f>
+      <c r="N14">
+        <f t="shared" ref="N14:N19" si="4">((0.5*25.5524)/(I14-H14))</f>
         <v>0.18408714320706596</v>
       </c>
-      <c r="M14">
-        <f t="shared" ref="M14:M19" si="3">(K14*J14)/I14</f>
+      <c r="O14">
+        <f t="shared" ref="O14:O19" si="5">(M14*L14)/K14</f>
         <v>3.4194450253305933E-2</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>0.5</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>6.8879999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -850,43 +895,51 @@
         <v>-6.8869999999999996</v>
       </c>
       <c r="F15">
+        <f t="shared" si="0"/>
+        <v>2.2470959280653329</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>2.5037614717013343</v>
+      </c>
+      <c r="H15">
         <v>11.832000000000001</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>82.117999999999995</v>
       </c>
-      <c r="H15">
-        <f xml:space="preserve"> (((D15-E15)/2)*25.5524)/(G15-F15)</f>
+      <c r="J15">
+        <f xml:space="preserve"> (((D15-E15)/2)*25.5524)/(I15-H15)</f>
         <v>2.3754286998833338</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <f xml:space="preserve"> (84.444 / 100*80.99)/85.25</f>
         <v>0.80224276363636371</v>
       </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>0.4412335200000001</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="1"/>
-        <v>6.1389865598130061E-2</v>
-      </c>
       <c r="L15">
         <f t="shared" si="2"/>
-        <v>0.18177446433144578</v>
+        <v>0.4412335200000001</v>
       </c>
       <c r="M15">
         <f t="shared" si="3"/>
+        <v>6.1389865598130061E-2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>0.18177446433144578</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="5"/>
         <v>3.3764426078971538E-2</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>0.5</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>6.8869999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -903,43 +956,51 @@
         <v>-6.7990000000000004</v>
       </c>
       <c r="F16">
+        <f t="shared" si="0"/>
+        <v>2.317246601055484</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>2.4779741491941238</v>
+      </c>
+      <c r="H16">
         <v>6.6219999999999999</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>76.731999999999999</v>
       </c>
-      <c r="H16">
-        <f xml:space="preserve"> (((D16-E16)/2)*25.5524)/(G16-F16)</f>
+      <c r="J16">
+        <f xml:space="preserve"> (((D16-E16)/2)*25.5524)/(I16-H16)</f>
         <v>2.3976103751248039</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <f xml:space="preserve"> (85.233 / 100*80.99)/85.25</f>
         <v>0.80973849501466266</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>0.44535617225806451</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="1"/>
-        <v>6.154431063423748E-2</v>
-      </c>
       <c r="L16">
         <f t="shared" si="2"/>
-        <v>0.18223078020253886</v>
+        <v>0.44535617225806451</v>
       </c>
       <c r="M16">
         <f t="shared" si="3"/>
+        <v>6.154431063423748E-2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>0.18223078020253886</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="5"/>
         <v>3.3849370848830621E-2</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>0.5</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>6.7990000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -956,43 +1017,51 @@
         <v>-5.9160000000000004</v>
       </c>
       <c r="F17">
+        <f t="shared" si="0"/>
+        <v>2.2605159160205588</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>2.1948485408136591</v>
+      </c>
+      <c r="H17">
         <v>4.8559999999999999</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>73.73</v>
       </c>
-      <c r="H17">
-        <f xml:space="preserve"> (((D17-E17)/2)*25.5524)/(G17-F17)</f>
+      <c r="J17">
+        <f xml:space="preserve"> (((D17-E17)/2)*25.5524)/(I17-H17)</f>
         <v>2.2276822284171094</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <f>(79.192/100*80.99)/85.25</f>
         <v>0.75234722346041039</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>0.41379097290322575</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>6.264861549341412E-2</v>
-      </c>
       <c r="L17">
         <f t="shared" si="2"/>
-        <v>0.18550105990649587</v>
+        <v>0.41379097290322575</v>
       </c>
       <c r="M17">
         <f t="shared" si="3"/>
+        <v>6.264861549341412E-2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>0.18550105990649587</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="5"/>
         <v>3.4456738521377768E-2</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>0.5</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>5.9160000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1009,43 +1078,51 @@
         <v>-5.298</v>
       </c>
       <c r="F18">
+        <f t="shared" si="0"/>
+        <v>1.9885223813510777</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>1.9885223813510777</v>
+      </c>
+      <c r="H18">
         <v>8.6530000000000005</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>76.731999999999999</v>
       </c>
-      <c r="H18">
-        <f xml:space="preserve"> (((D18-E18)/2)*25.5524)/(G18-F18)</f>
+      <c r="J18">
+        <f xml:space="preserve"> (((D18-E18)/2)*25.5524)/(I18-H18)</f>
         <v>1.9885223813510777</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <f>(70.69/100*80.99)/85.25</f>
         <v>0.6715757302052785</v>
       </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>0.36936665161290322</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
-        <v>6.3380117988418125E-2</v>
-      </c>
       <c r="L18">
         <f t="shared" si="2"/>
-        <v>0.18766726890818022</v>
+        <v>0.36936665161290322</v>
       </c>
       <c r="M18">
         <f t="shared" si="3"/>
+        <v>6.3380117988418125E-2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>0.18766726890818022</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="5"/>
         <v>3.4859064893629978E-2</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>0.5</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>5.298</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1062,39 +1139,47 @@
         <v>-4.68</v>
       </c>
       <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1.8744658747394658</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>1.7429962832864494</v>
+      </c>
+      <c r="H19">
         <v>6.6219999999999999</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>75.230999999999995</v>
       </c>
-      <c r="H19">
-        <f xml:space="preserve"> (((D19-E19)/2)*25.5524)/(G19-F19)</f>
+      <c r="J19">
+        <f xml:space="preserve"> (((D19-E19)/2)*25.5524)/(I19-H19)</f>
         <v>1.8087310790129578</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <f>61.086/100</f>
         <v>0.61085999999999996</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>0.33597300000000002</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="1"/>
-        <v>6.2890970863790779E-2</v>
-      </c>
       <c r="L19">
         <f t="shared" si="2"/>
-        <v>0.18621755163316767</v>
+        <v>0.33597300000000002</v>
       </c>
       <c r="M19">
         <f t="shared" si="3"/>
+        <v>6.2890970863790779E-2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="4"/>
+        <v>0.18621755163316767</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="5"/>
         <v>3.4590033975084936E-2</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>0.5</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>4.68</v>
       </c>
     </row>

</xml_diff>